<commit_message>
add new chinese lessons 20200411
</commit_message>
<xml_diff>
--- a/learn_chinese.xlsx
+++ b/learn_chinese.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DCD2D7-1A7E-4B53-A9A0-B26320F6E79C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0D6FEA-1B38-45C3-9FAD-B4F9D12C36A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="22" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="23" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20190323" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="20200321" sheetId="30" r:id="rId26"/>
     <sheet name="20200328" sheetId="32" r:id="rId27"/>
     <sheet name="20200404" sheetId="33" r:id="rId28"/>
+    <sheet name="20200411" sheetId="34" r:id="rId29"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1776" uniqueCount="1688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="1731">
   <si>
     <t>1. Some simple chinese word</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39560,6 +39561,1131 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> some paper spiritual money to ancestors.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: 最近怎么样。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: 你怎么知道的？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C: 把你的症状告诉我。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: What's going on?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: How do you know?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C: Please tell me about your symptoms.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zuì jìn zěn me yàng 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>没什么新鲜</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>老样子</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。为什么这么问？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nothing much</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>just the usual</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Why do you ask?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>méi shí me xīn xiān de</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">lǎo yàng zǐ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。wéi shí me zhè me wèn ？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nǐ zěn me zhī dào de ？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bǎ nǐ de zhèng zhuàng gào sù wǒ 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 你在</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>流鼻涕</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，你看起来像是在</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>发烧</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: Your </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nose is running</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and you seem like you </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>have a fever</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nǐ zài </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>liú bí tì</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ，nǐ kàn qǐ lái xiàng shì zài</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fā shāo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 从你的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>症状</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>看出来的，我们应该去</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>看医生</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: I can see </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>your symptoms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. We should go to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> see a doctor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cóng nǐ de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>zhèng zhuàng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> kàn chū lái de ，wǒ men yīng gāi qù </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kàn yī shēng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 太好了，我</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>希望</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>那个说英语的医生能帮我。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: Great, I </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hope</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the English-speaking doctor can help me.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">tài hǎo le ，wǒ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>xī wàng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nà gè shuō yīng yǔ de yī shēng néng bāng wǒ 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: My nose is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>constantly</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> running. I have a fever and I vomited a few times. </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 我</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>老</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>是流鼻涕，发烧，你觉得我是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>感冒</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>吗？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">wǒ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">lǎo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">shì liú bí tì ，fā shāo ，nǐ jiào dé wǒ shì </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gǎn mào</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ma ？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Do you think it is a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>C: 不是，我想可能是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>流感</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>C: Sorry to say, no. I think it might be the</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> flu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">bú shì ，wǒ xiǎng kě néng shì </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>liú gǎn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 流感比感冒更</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>严重</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>吗？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">liú gǎn bǐ gǎn mào gèng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yán zhòng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ma ？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: Is the flu more </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>serious</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> than a cold?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>C: 是的，流感</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>四处传播</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，更糟糕。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C: Correct. The flu that is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>going around</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is rather bad.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">shì de ，liú gǎn </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sì chù chuán bō</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ，gèng zāo gāo 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 我的朋友玛丽昨天也发烧了，是她</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>传染</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>给我的吗？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: My friend Mary was also have a fever, Do you think she </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gave</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the flu to me?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>C: 可能，你应该</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>尽快</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>来</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>医院</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C: Maybe, you should come into the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hospital</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>as soon as possible</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>kě néng ，nǐ yīng gāi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jìn kuài</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lái </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yī yuàn</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>See the doctor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">我吐了， wǒ tǔ le </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> I vomited</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">wǒ de péng yǒu Mary zuó tiān yě fā shāo le  ，shì tā </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>chuán rǎn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> gěi wǒ de ma ？</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -52365,7 +53491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D144B9A3-748C-407B-935D-62605552AB90}">
   <dimension ref="C3:BE56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -52958,6 +54084,604 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D02019-92B0-4E22-AD62-F1F59CBAB36F}">
+  <dimension ref="C3:BG49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB20" sqref="AB20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.640625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="8" width="2.640625" style="29"/>
+    <col min="9" max="9" width="2.7109375" style="29" customWidth="1"/>
+    <col min="10" max="15" width="2.640625" style="29"/>
+    <col min="16" max="16" width="2.640625" style="29" customWidth="1"/>
+    <col min="17" max="35" width="2.640625" style="29"/>
+    <col min="36" max="36" width="2.640625" style="29" customWidth="1"/>
+    <col min="37" max="38" width="2.640625" style="29"/>
+    <col min="39" max="39" width="2.640625" style="29" customWidth="1"/>
+    <col min="40" max="16384" width="2.640625" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="C3" s="29" t="s">
+        <v>628</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="I3" s="30"/>
+      <c r="AF3" s="23"/>
+    </row>
+    <row r="4" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="D4" s="23" t="s">
+        <v>1727</v>
+      </c>
+      <c r="I4" s="30"/>
+      <c r="AF4" s="23"/>
+    </row>
+    <row r="5" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="C5" s="29" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="AC5" s="29" t="s">
+        <v>1691</v>
+      </c>
+      <c r="AF5" s="23"/>
+    </row>
+    <row r="6" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="D6" s="29" t="s">
+        <v>1694</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
+      <c r="X6" s="30"/>
+      <c r="Y6" s="30"/>
+      <c r="Z6" s="30"/>
+      <c r="AA6" s="30"/>
+      <c r="AB6" s="30"/>
+      <c r="AC6" s="30"/>
+      <c r="AD6" s="30"/>
+      <c r="AE6" s="30"/>
+      <c r="AF6" s="30"/>
+    </row>
+    <row r="7" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="C7" s="29" t="s">
+        <v>1695</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="AC7" s="29" t="s">
+        <v>1696</v>
+      </c>
+      <c r="AF7" s="23"/>
+    </row>
+    <row r="8" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="D8" s="23" t="s">
+        <v>1697</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="AF8" s="23"/>
+      <c r="AM8" s="33"/>
+    </row>
+    <row r="9" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="C9" s="29" t="s">
+        <v>1700</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="AC9" s="29" t="s">
+        <v>1701</v>
+      </c>
+      <c r="AF9" s="23"/>
+      <c r="AM9" s="33"/>
+    </row>
+    <row r="10" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="D10" s="23" t="s">
+        <v>1702</v>
+      </c>
+      <c r="E10" s="23"/>
+      <c r="AF10" s="23"/>
+      <c r="AM10" s="33"/>
+      <c r="AN10" s="32"/>
+    </row>
+    <row r="11" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="C11" s="29" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="AC11" s="29" t="s">
+        <v>1692</v>
+      </c>
+      <c r="AF11" s="23"/>
+      <c r="AM11" s="33"/>
+      <c r="AN11" s="32"/>
+      <c r="AP11" s="23"/>
+    </row>
+    <row r="12" spans="3:43" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="23" t="s">
+        <v>1698</v>
+      </c>
+      <c r="E12" s="23"/>
+      <c r="AF12" s="23"/>
+      <c r="AM12" s="33"/>
+      <c r="AN12" s="32"/>
+    </row>
+    <row r="13" spans="3:43" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="29" t="s">
+        <v>1703</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="AC13" s="29" t="s">
+        <v>1704</v>
+      </c>
+      <c r="AF13" s="23"/>
+      <c r="AM13" s="33"/>
+      <c r="AN13" s="32"/>
+    </row>
+    <row r="14" spans="3:43" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="23" t="s">
+        <v>1705</v>
+      </c>
+      <c r="E14" s="23"/>
+      <c r="AF14" s="23"/>
+      <c r="AM14" s="33"/>
+      <c r="AN14" s="32"/>
+    </row>
+    <row r="15" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="C15" s="29" t="s">
+        <v>1706</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="AC15" s="29" t="s">
+        <v>1707</v>
+      </c>
+      <c r="AF15" s="23"/>
+      <c r="AM15" s="33"/>
+      <c r="AQ15" s="23"/>
+    </row>
+    <row r="16" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="D16" s="23" t="s">
+        <v>1708</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="AF16" s="23"/>
+      <c r="AK16" s="23"/>
+      <c r="AM16" s="33"/>
+      <c r="AN16" s="32"/>
+      <c r="AQ16" s="23"/>
+    </row>
+    <row r="17" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="C17" s="29" t="s">
+        <v>1690</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="AC17" s="29" t="s">
+        <v>1693</v>
+      </c>
+      <c r="AF17" s="23"/>
+      <c r="AK17" s="23"/>
+      <c r="AM17" s="33"/>
+      <c r="AN17" s="32"/>
+      <c r="AQ17" s="23"/>
+    </row>
+    <row r="18" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="D18" s="23" t="s">
+        <v>1699</v>
+      </c>
+      <c r="E18" s="23"/>
+      <c r="AF18" s="23"/>
+      <c r="AK18" s="23"/>
+      <c r="AM18" s="33"/>
+      <c r="AN18" s="32"/>
+      <c r="AQ18" s="23"/>
+    </row>
+    <row r="19" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="C19" s="29" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="AC19" s="29" t="s">
+        <v>1709</v>
+      </c>
+      <c r="AF19" s="23"/>
+      <c r="AM19" s="33"/>
+      <c r="AQ19" s="23"/>
+    </row>
+    <row r="20" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="D20" s="23" t="s">
+        <v>1711</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="AD20" s="29" t="s">
+        <v>1712</v>
+      </c>
+      <c r="AF20" s="23"/>
+      <c r="AM20" s="33"/>
+      <c r="AN20" s="32"/>
+      <c r="AQ20" s="23"/>
+    </row>
+    <row r="21" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="C21" s="29" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E21" s="23"/>
+      <c r="AC21" s="29" t="s">
+        <v>1714</v>
+      </c>
+      <c r="AL21" s="32"/>
+      <c r="AQ21" s="23"/>
+    </row>
+    <row r="22" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="D22" s="29" t="s">
+        <v>1715</v>
+      </c>
+      <c r="E22" s="23"/>
+      <c r="AL22" s="32"/>
+      <c r="AQ22" s="23"/>
+    </row>
+    <row r="23" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="C23" s="29" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E23" s="23"/>
+      <c r="AC23" s="29" t="s">
+        <v>1718</v>
+      </c>
+      <c r="AL23" s="32"/>
+      <c r="AQ23" s="23"/>
+    </row>
+    <row r="24" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="D24" s="23" t="s">
+        <v>1717</v>
+      </c>
+      <c r="E24" s="23"/>
+      <c r="AL24" s="32"/>
+      <c r="AQ24" s="23"/>
+    </row>
+    <row r="25" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="C25" s="29" t="s">
+        <v>1719</v>
+      </c>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="AC25" s="29" t="s">
+        <v>1720</v>
+      </c>
+      <c r="AL25" s="32"/>
+      <c r="AQ25" s="23"/>
+    </row>
+    <row r="26" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="D26" s="23" t="s">
+        <v>1721</v>
+      </c>
+      <c r="E26" s="23"/>
+      <c r="AK26" s="23"/>
+      <c r="AL26" s="32"/>
+      <c r="AQ26" s="23"/>
+    </row>
+    <row r="27" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="C27" s="29" t="s">
+        <v>1722</v>
+      </c>
+      <c r="AC27" s="29" t="s">
+        <v>1723</v>
+      </c>
+      <c r="AK27" s="23"/>
+      <c r="AL27" s="32"/>
+      <c r="AQ27" s="23"/>
+    </row>
+    <row r="28" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="D28" s="23" t="s">
+        <v>1730</v>
+      </c>
+      <c r="AL28" s="32"/>
+      <c r="AQ28" s="23"/>
+    </row>
+    <row r="29" spans="3:43" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="29" t="s">
+        <v>1724</v>
+      </c>
+      <c r="E29" s="23"/>
+      <c r="AC29" s="29" t="s">
+        <v>1725</v>
+      </c>
+      <c r="AL29" s="32"/>
+      <c r="AQ29" s="23"/>
+    </row>
+    <row r="30" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="D30" s="29" t="s">
+        <v>1726</v>
+      </c>
+      <c r="E30" s="23"/>
+      <c r="AK30" s="23"/>
+      <c r="AL30" s="32"/>
+      <c r="AQ30" s="23"/>
+    </row>
+    <row r="31" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="E31" s="23"/>
+      <c r="AQ31" s="23"/>
+    </row>
+    <row r="32" spans="3:43" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E32" s="23"/>
+      <c r="AQ32" s="23"/>
+    </row>
+    <row r="33" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="C33" s="29" t="s">
+        <v>1728</v>
+      </c>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="J33" s="29" t="s">
+        <v>1729</v>
+      </c>
+      <c r="AM33" s="23"/>
+    </row>
+    <row r="34" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="AM34" s="23"/>
+    </row>
+    <row r="35" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="AM35" s="23"/>
+    </row>
+    <row r="36" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="D36" s="23"/>
+    </row>
+    <row r="37" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="E37" s="23"/>
+      <c r="AM37" s="23"/>
+    </row>
+    <row r="38" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="E38" s="23"/>
+    </row>
+    <row r="39" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
+      <c r="AG39" s="23"/>
+      <c r="AH39" s="23"/>
+      <c r="AI39" s="23"/>
+      <c r="AN39" s="23"/>
+      <c r="AO39" s="23"/>
+      <c r="AP39" s="23"/>
+      <c r="AQ39" s="23"/>
+      <c r="AR39" s="23"/>
+      <c r="AS39" s="23"/>
+      <c r="AT39" s="23"/>
+      <c r="AU39" s="23"/>
+      <c r="AV39" s="23"/>
+      <c r="AW39" s="23"/>
+    </row>
+    <row r="40" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="23"/>
+      <c r="P40" s="32"/>
+      <c r="Q40" s="32"/>
+      <c r="R40" s="32"/>
+      <c r="S40" s="32"/>
+      <c r="T40" s="32"/>
+      <c r="U40" s="32"/>
+      <c r="V40" s="32"/>
+      <c r="W40" s="32"/>
+      <c r="X40" s="32"/>
+      <c r="Y40" s="32"/>
+      <c r="Z40" s="32"/>
+      <c r="AA40" s="32"/>
+      <c r="AB40" s="32"/>
+      <c r="AC40" s="32"/>
+      <c r="AD40" s="32"/>
+      <c r="AE40" s="32"/>
+      <c r="AG40" s="23"/>
+      <c r="AH40" s="23"/>
+      <c r="AI40" s="23"/>
+      <c r="AN40" s="23"/>
+      <c r="AO40" s="23"/>
+      <c r="AP40" s="23"/>
+      <c r="AQ40" s="23"/>
+      <c r="AR40" s="23"/>
+      <c r="AS40" s="23"/>
+      <c r="AT40" s="23"/>
+      <c r="AU40" s="23"/>
+      <c r="AV40" s="23"/>
+      <c r="AW40" s="23"/>
+    </row>
+    <row r="41" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="C41" s="38"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="23"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="S41" s="32"/>
+      <c r="T41" s="32"/>
+      <c r="U41" s="32"/>
+      <c r="V41" s="32"/>
+      <c r="W41" s="32"/>
+      <c r="X41" s="32"/>
+      <c r="Y41" s="32"/>
+      <c r="Z41" s="32"/>
+      <c r="AA41" s="32"/>
+      <c r="AB41" s="32"/>
+      <c r="AC41" s="32"/>
+      <c r="AD41" s="32"/>
+      <c r="AE41" s="32"/>
+      <c r="AG41" s="23"/>
+      <c r="AH41" s="23"/>
+      <c r="AI41" s="23"/>
+      <c r="AN41" s="23"/>
+      <c r="AO41" s="23"/>
+      <c r="AP41" s="23"/>
+      <c r="AQ41" s="23"/>
+      <c r="AR41" s="23"/>
+      <c r="AS41" s="23"/>
+      <c r="AT41" s="23"/>
+      <c r="AU41" s="23"/>
+      <c r="AV41" s="23"/>
+      <c r="AW41" s="23"/>
+    </row>
+    <row r="42" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="M42" s="23"/>
+      <c r="N42" s="23"/>
+      <c r="O42" s="23"/>
+      <c r="AL42" s="23"/>
+      <c r="AM42" s="23"/>
+      <c r="AN42" s="23"/>
+      <c r="AO42" s="23"/>
+      <c r="AP42" s="23"/>
+      <c r="AQ42" s="23"/>
+      <c r="AR42" s="23"/>
+      <c r="AS42" s="23"/>
+      <c r="AT42" s="23"/>
+      <c r="AU42" s="23"/>
+      <c r="AV42" s="23"/>
+      <c r="AW42" s="23"/>
+      <c r="BE42" s="23"/>
+      <c r="BF42" s="23"/>
+      <c r="BG42" s="23"/>
+    </row>
+    <row r="43" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="23"/>
+      <c r="AL43" s="23"/>
+      <c r="AM43" s="23"/>
+      <c r="AN43" s="23"/>
+      <c r="AO43" s="23"/>
+      <c r="AP43" s="23"/>
+      <c r="AQ43" s="23"/>
+      <c r="AR43" s="23"/>
+      <c r="AS43" s="23"/>
+      <c r="AT43" s="23"/>
+      <c r="AU43" s="23"/>
+      <c r="AV43" s="23"/>
+      <c r="AW43" s="23"/>
+      <c r="BE43" s="23"/>
+      <c r="BF43" s="23"/>
+      <c r="BG43" s="23"/>
+    </row>
+    <row r="44" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="M44" s="23"/>
+      <c r="N44" s="23"/>
+      <c r="O44" s="23"/>
+      <c r="AL44" s="23"/>
+      <c r="AM44" s="23"/>
+      <c r="AN44" s="23"/>
+      <c r="AO44" s="23"/>
+      <c r="AP44" s="23"/>
+      <c r="AQ44" s="23"/>
+      <c r="AR44" s="23"/>
+      <c r="AS44" s="23"/>
+      <c r="AT44" s="23"/>
+      <c r="AU44" s="23"/>
+      <c r="AV44" s="23"/>
+      <c r="AW44" s="23"/>
+    </row>
+    <row r="45" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
+      <c r="O45" s="23"/>
+      <c r="AL45" s="23"/>
+      <c r="AM45" s="23"/>
+      <c r="AN45" s="23"/>
+      <c r="AO45" s="23"/>
+      <c r="AP45" s="23"/>
+      <c r="AQ45" s="23"/>
+      <c r="AR45" s="23"/>
+      <c r="AS45" s="23"/>
+      <c r="AT45" s="23"/>
+      <c r="AU45" s="23"/>
+      <c r="AV45" s="23"/>
+      <c r="AW45" s="23"/>
+    </row>
+    <row r="46" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="AN46" s="23"/>
+      <c r="AO46" s="23"/>
+      <c r="AP46" s="23"/>
+      <c r="AQ46" s="23"/>
+      <c r="AR46" s="23"/>
+      <c r="AS46" s="23"/>
+      <c r="AT46" s="23"/>
+      <c r="AU46" s="23"/>
+      <c r="AV46" s="23"/>
+      <c r="AW46" s="23"/>
+      <c r="BA46" s="36"/>
+    </row>
+    <row r="47" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="AN47" s="23"/>
+      <c r="AO47" s="23"/>
+      <c r="AP47" s="23"/>
+      <c r="AQ47" s="23"/>
+      <c r="AR47" s="23"/>
+      <c r="AS47" s="23"/>
+      <c r="AT47" s="23"/>
+      <c r="AU47" s="23"/>
+      <c r="AV47" s="23"/>
+      <c r="AW47" s="23"/>
+      <c r="BA47" s="36"/>
+    </row>
+    <row r="48" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="AN48" s="23"/>
+      <c r="AO48" s="23"/>
+      <c r="AP48" s="23"/>
+      <c r="AQ48" s="23"/>
+      <c r="AR48" s="23"/>
+      <c r="AS48" s="23"/>
+      <c r="AT48" s="23"/>
+      <c r="AU48" s="23"/>
+      <c r="AV48" s="23"/>
+      <c r="AW48" s="23"/>
+    </row>
+    <row r="49" spans="3:49" x14ac:dyDescent="0.35">
+      <c r="C49" s="36"/>
+      <c r="AN49" s="23"/>
+      <c r="AO49" s="23"/>
+      <c r="AP49" s="23"/>
+      <c r="AQ49" s="23"/>
+      <c r="AR49" s="23"/>
+      <c r="AS49" s="23"/>
+      <c r="AT49" s="23"/>
+      <c r="AU49" s="23"/>
+      <c r="AV49" s="23"/>
+      <c r="AW49" s="23"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:AF23"/>

</xml_diff>

<commit_message>
add new chinese lessons
</commit_message>
<xml_diff>
--- a/learn_chinese.xlsx
+++ b/learn_chinese.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0D6FEA-1B38-45C3-9FAD-B4F9D12C36A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B8323E-93BD-4C0B-B754-11DD13513A5C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="23" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="24" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20190323" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <sheet name="20200328" sheetId="32" r:id="rId27"/>
     <sheet name="20200404" sheetId="33" r:id="rId28"/>
     <sheet name="20200411" sheetId="34" r:id="rId29"/>
+    <sheet name="20200418" sheetId="35" r:id="rId30"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="1731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="1764">
   <si>
     <t>1. Some simple chinese word</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -40687,6 +40688,136 @@
       </rPr>
       <t xml:space="preserve"> gěi wǒ de ma ？</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>古诗两首</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>草</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>唐代：白居易</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>离离原上草，一岁一枯荣。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>野火烧不尽，春风吹又生。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>赠汪伦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>唐代：李白</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李白乘舟将欲行，忽闻岸上踏歌声。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">cǎo </t>
+  </si>
+  <si>
+    <t>táng dài ：bái jū yì</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lí lí yuán shàng cǎo ，yī suì yī kū róng 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yě huǒ shāo bú jìn ，chūn fēng chuī yòu shēng 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">zèng wāng lún </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lǐ bái chéng zhōu jiāng yù xing，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hū wén àn shàng tà gē shēng 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bú jí wāng lún sòng wǒ qíng 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">gǔ shī liǎng shǒu </t>
+  </si>
+  <si>
+    <t>two ancient poetry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the Tang Dynasty: bái jū yì</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The grass is thick on the grassland,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Once a year there is an alternation of blight and flourish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wild fire can't burn up  them,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>They will grow out when the spring wind comes.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>táng dài ：lǐ bái</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the Tang Dynasty: lǐ bái</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Present Wang Lun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桃花潭水深千尺，不及汪伦送我情。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li bai wants to travel by boat，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The peach blossom pool depth thousand feet,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> less than Wang Lun send me.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Suddenly he head singing and dancing in the bank.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>táo huā tán shuǐ shen qiān chǐ ，</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -54088,7 +54219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D02019-92B0-4E22-AD62-F1F59CBAB36F}">
   <dimension ref="C3:BG49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
@@ -55002,6 +55133,585 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B76428C-87A1-4667-BACC-1B380355DDA5}">
+  <dimension ref="B3:BG50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.640625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="8" width="2.640625" style="29"/>
+    <col min="9" max="9" width="2.7109375" style="29" customWidth="1"/>
+    <col min="10" max="15" width="2.640625" style="29"/>
+    <col min="16" max="16" width="2.640625" style="29" customWidth="1"/>
+    <col min="17" max="35" width="2.640625" style="29"/>
+    <col min="36" max="36" width="2.640625" style="29" customWidth="1"/>
+    <col min="37" max="38" width="2.640625" style="29"/>
+    <col min="39" max="39" width="2.640625" style="29" customWidth="1"/>
+    <col min="40" max="16384" width="2.640625" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="C3" s="29" t="s">
+        <v>628</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="I3" s="30"/>
+      <c r="AF3" s="23"/>
+    </row>
+    <row r="4" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="D4" s="23"/>
+      <c r="I4" s="30"/>
+      <c r="AF4" s="23"/>
+    </row>
+    <row r="5" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="D5" s="23" t="s">
+        <v>1731</v>
+      </c>
+      <c r="E5" s="30"/>
+      <c r="H5" s="29" t="s">
+        <v>1747</v>
+      </c>
+      <c r="I5" s="30"/>
+      <c r="AE5" s="29" t="s">
+        <v>1748</v>
+      </c>
+      <c r="AF5" s="23"/>
+    </row>
+    <row r="6" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="E6" s="23"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
+      <c r="X6" s="30"/>
+      <c r="Y6" s="30"/>
+      <c r="Z6" s="30"/>
+      <c r="AA6" s="30"/>
+      <c r="AB6" s="30"/>
+      <c r="AC6" s="30"/>
+      <c r="AD6" s="30"/>
+      <c r="AE6" s="30"/>
+      <c r="AF6" s="30"/>
+    </row>
+    <row r="7" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="E7" s="23" t="s">
+        <v>1732</v>
+      </c>
+      <c r="AF7" s="23" t="s">
+        <v>1749</v>
+      </c>
+      <c r="AM7" s="33"/>
+    </row>
+    <row r="8" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="C8" s="29" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="AD8" s="29" t="s">
+        <v>1750</v>
+      </c>
+      <c r="AF8" s="23"/>
+      <c r="AM8" s="33"/>
+    </row>
+    <row r="9" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="B9" s="29" t="s">
+        <v>1734</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="AB9" s="29" t="s">
+        <v>1751</v>
+      </c>
+      <c r="AF9" s="23"/>
+      <c r="AM9" s="33"/>
+      <c r="AN9" s="32"/>
+    </row>
+    <row r="10" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="B10" s="29" t="s">
+        <v>1735</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="AB10" s="29" t="s">
+        <v>1752</v>
+      </c>
+      <c r="AF10" s="23"/>
+      <c r="AM10" s="33"/>
+      <c r="AN10" s="32"/>
+      <c r="AP10" s="23"/>
+    </row>
+    <row r="11" spans="2:43" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="23"/>
+      <c r="E11" s="23" t="s">
+        <v>1739</v>
+      </c>
+      <c r="AB11" s="29" t="s">
+        <v>1753</v>
+      </c>
+      <c r="AF11" s="23"/>
+      <c r="AM11" s="33"/>
+      <c r="AN11" s="32"/>
+    </row>
+    <row r="12" spans="2:43" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="29" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="AB12" s="29" t="s">
+        <v>1754</v>
+      </c>
+      <c r="AF12" s="23"/>
+      <c r="AM12" s="33"/>
+      <c r="AN12" s="32"/>
+    </row>
+    <row r="13" spans="2:43" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="29" t="s">
+        <v>1741</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="AF13" s="23"/>
+      <c r="AM13" s="33"/>
+      <c r="AN13" s="32"/>
+    </row>
+    <row r="14" spans="2:43" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="29" t="s">
+        <v>1742</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="AF14" s="23"/>
+      <c r="AM14" s="33"/>
+      <c r="AN14" s="32"/>
+    </row>
+    <row r="15" spans="2:43" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AF15" s="23"/>
+      <c r="AM15" s="33"/>
+      <c r="AN15" s="32"/>
+    </row>
+    <row r="16" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="AF16" s="23"/>
+      <c r="AM16" s="33"/>
+      <c r="AQ16" s="23"/>
+    </row>
+    <row r="17" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="D17" s="23" t="s">
+        <v>1736</v>
+      </c>
+      <c r="E17" s="23"/>
+      <c r="AE17" s="29" t="s">
+        <v>1757</v>
+      </c>
+      <c r="AF17" s="23"/>
+      <c r="AK17" s="23"/>
+      <c r="AM17" s="33"/>
+      <c r="AN17" s="32"/>
+      <c r="AQ17" s="23"/>
+    </row>
+    <row r="18" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="C18" s="23" t="s">
+        <v>1737</v>
+      </c>
+      <c r="E18" s="23"/>
+      <c r="AD18" s="29" t="s">
+        <v>1756</v>
+      </c>
+      <c r="AF18" s="23"/>
+      <c r="AK18" s="23"/>
+      <c r="AM18" s="33"/>
+      <c r="AN18" s="32"/>
+      <c r="AQ18" s="23"/>
+    </row>
+    <row r="19" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="B19" s="29" t="s">
+        <v>1738</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="AB19" s="29" t="s">
+        <v>1759</v>
+      </c>
+      <c r="AF19" s="23"/>
+      <c r="AK19" s="23"/>
+      <c r="AM19" s="33"/>
+      <c r="AN19" s="32"/>
+      <c r="AQ19" s="23"/>
+    </row>
+    <row r="20" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="B20" s="29" t="s">
+        <v>1758</v>
+      </c>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="AB20" s="29" t="s">
+        <v>1762</v>
+      </c>
+      <c r="AF20" s="23"/>
+      <c r="AM20" s="33"/>
+      <c r="AQ20" s="23"/>
+    </row>
+    <row r="21" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="D21" s="23" t="s">
+        <v>1743</v>
+      </c>
+      <c r="E21" s="23"/>
+      <c r="AB21" s="29" t="s">
+        <v>1760</v>
+      </c>
+      <c r="AF21" s="23"/>
+      <c r="AM21" s="33"/>
+      <c r="AN21" s="32"/>
+      <c r="AQ21" s="23"/>
+    </row>
+    <row r="22" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="B22" s="29" t="s">
+        <v>1755</v>
+      </c>
+      <c r="E22" s="23"/>
+      <c r="AB22" s="29" t="s">
+        <v>1761</v>
+      </c>
+      <c r="AL22" s="32"/>
+      <c r="AQ22" s="23"/>
+    </row>
+    <row r="23" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="B23" s="29" t="s">
+        <v>1744</v>
+      </c>
+      <c r="E23" s="23"/>
+      <c r="AL23" s="32"/>
+      <c r="AQ23" s="23"/>
+    </row>
+    <row r="24" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="B24" s="29" t="s">
+        <v>1745</v>
+      </c>
+      <c r="E24" s="23"/>
+      <c r="AL24" s="32"/>
+      <c r="AQ24" s="23"/>
+    </row>
+    <row r="25" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="B25" s="29" t="s">
+        <v>1763</v>
+      </c>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="AL25" s="32"/>
+      <c r="AQ25" s="23"/>
+    </row>
+    <row r="26" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="B26" s="29" t="s">
+        <v>1746</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="AL26" s="32"/>
+      <c r="AQ26" s="23"/>
+    </row>
+    <row r="27" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="AK27" s="23"/>
+      <c r="AL27" s="32"/>
+      <c r="AQ27" s="23"/>
+    </row>
+    <row r="28" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="AK28" s="23"/>
+      <c r="AL28" s="32"/>
+      <c r="AQ28" s="23"/>
+    </row>
+    <row r="29" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="D29" s="23"/>
+      <c r="AL29" s="32"/>
+      <c r="AQ29" s="23"/>
+    </row>
+    <row r="30" spans="2:43" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E30" s="23"/>
+      <c r="AL30" s="32"/>
+      <c r="AQ30" s="23"/>
+    </row>
+    <row r="31" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="E31" s="23"/>
+      <c r="AK31" s="23"/>
+      <c r="AL31" s="32"/>
+      <c r="AQ31" s="23"/>
+    </row>
+    <row r="32" spans="2:43" x14ac:dyDescent="0.35">
+      <c r="E32" s="23"/>
+      <c r="AQ32" s="23"/>
+    </row>
+    <row r="33" spans="3:59" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E33" s="23"/>
+      <c r="AQ33" s="23"/>
+    </row>
+    <row r="34" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="AM34" s="23"/>
+    </row>
+    <row r="35" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="AM35" s="23"/>
+    </row>
+    <row r="36" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="AM36" s="23"/>
+    </row>
+    <row r="37" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="D37" s="23"/>
+    </row>
+    <row r="38" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="E38" s="23"/>
+      <c r="AM38" s="23"/>
+    </row>
+    <row r="39" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="E39" s="23"/>
+    </row>
+    <row r="40" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
+      <c r="AG40" s="23"/>
+      <c r="AH40" s="23"/>
+      <c r="AI40" s="23"/>
+      <c r="AN40" s="23"/>
+      <c r="AO40" s="23"/>
+      <c r="AP40" s="23"/>
+      <c r="AQ40" s="23"/>
+      <c r="AR40" s="23"/>
+      <c r="AS40" s="23"/>
+      <c r="AT40" s="23"/>
+      <c r="AU40" s="23"/>
+      <c r="AV40" s="23"/>
+      <c r="AW40" s="23"/>
+    </row>
+    <row r="41" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="23"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="S41" s="32"/>
+      <c r="T41" s="32"/>
+      <c r="U41" s="32"/>
+      <c r="V41" s="32"/>
+      <c r="W41" s="32"/>
+      <c r="X41" s="32"/>
+      <c r="Y41" s="32"/>
+      <c r="Z41" s="32"/>
+      <c r="AA41" s="32"/>
+      <c r="AB41" s="32"/>
+      <c r="AC41" s="32"/>
+      <c r="AD41" s="32"/>
+      <c r="AE41" s="32"/>
+      <c r="AG41" s="23"/>
+      <c r="AH41" s="23"/>
+      <c r="AI41" s="23"/>
+      <c r="AN41" s="23"/>
+      <c r="AO41" s="23"/>
+      <c r="AP41" s="23"/>
+      <c r="AQ41" s="23"/>
+      <c r="AR41" s="23"/>
+      <c r="AS41" s="23"/>
+      <c r="AT41" s="23"/>
+      <c r="AU41" s="23"/>
+      <c r="AV41" s="23"/>
+      <c r="AW41" s="23"/>
+    </row>
+    <row r="42" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="C42" s="38"/>
+      <c r="M42" s="23"/>
+      <c r="N42" s="23"/>
+      <c r="O42" s="23"/>
+      <c r="P42" s="32"/>
+      <c r="Q42" s="32"/>
+      <c r="R42" s="32"/>
+      <c r="S42" s="32"/>
+      <c r="T42" s="32"/>
+      <c r="U42" s="32"/>
+      <c r="V42" s="32"/>
+      <c r="W42" s="32"/>
+      <c r="X42" s="32"/>
+      <c r="Y42" s="32"/>
+      <c r="Z42" s="32"/>
+      <c r="AA42" s="32"/>
+      <c r="AB42" s="32"/>
+      <c r="AC42" s="32"/>
+      <c r="AD42" s="32"/>
+      <c r="AE42" s="32"/>
+      <c r="AG42" s="23"/>
+      <c r="AH42" s="23"/>
+      <c r="AI42" s="23"/>
+      <c r="AN42" s="23"/>
+      <c r="AO42" s="23"/>
+      <c r="AP42" s="23"/>
+      <c r="AQ42" s="23"/>
+      <c r="AR42" s="23"/>
+      <c r="AS42" s="23"/>
+      <c r="AT42" s="23"/>
+      <c r="AU42" s="23"/>
+      <c r="AV42" s="23"/>
+      <c r="AW42" s="23"/>
+    </row>
+    <row r="43" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="23"/>
+      <c r="AL43" s="23"/>
+      <c r="AM43" s="23"/>
+      <c r="AN43" s="23"/>
+      <c r="AO43" s="23"/>
+      <c r="AP43" s="23"/>
+      <c r="AQ43" s="23"/>
+      <c r="AR43" s="23"/>
+      <c r="AS43" s="23"/>
+      <c r="AT43" s="23"/>
+      <c r="AU43" s="23"/>
+      <c r="AV43" s="23"/>
+      <c r="AW43" s="23"/>
+      <c r="BE43" s="23"/>
+      <c r="BF43" s="23"/>
+      <c r="BG43" s="23"/>
+    </row>
+    <row r="44" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="M44" s="23"/>
+      <c r="N44" s="23"/>
+      <c r="O44" s="23"/>
+      <c r="AL44" s="23"/>
+      <c r="AM44" s="23"/>
+      <c r="AN44" s="23"/>
+      <c r="AO44" s="23"/>
+      <c r="AP44" s="23"/>
+      <c r="AQ44" s="23"/>
+      <c r="AR44" s="23"/>
+      <c r="AS44" s="23"/>
+      <c r="AT44" s="23"/>
+      <c r="AU44" s="23"/>
+      <c r="AV44" s="23"/>
+      <c r="AW44" s="23"/>
+      <c r="BE44" s="23"/>
+      <c r="BF44" s="23"/>
+      <c r="BG44" s="23"/>
+    </row>
+    <row r="45" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
+      <c r="O45" s="23"/>
+      <c r="AL45" s="23"/>
+      <c r="AM45" s="23"/>
+      <c r="AN45" s="23"/>
+      <c r="AO45" s="23"/>
+      <c r="AP45" s="23"/>
+      <c r="AQ45" s="23"/>
+      <c r="AR45" s="23"/>
+      <c r="AS45" s="23"/>
+      <c r="AT45" s="23"/>
+      <c r="AU45" s="23"/>
+      <c r="AV45" s="23"/>
+      <c r="AW45" s="23"/>
+    </row>
+    <row r="46" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
+      <c r="O46" s="23"/>
+      <c r="AL46" s="23"/>
+      <c r="AM46" s="23"/>
+      <c r="AN46" s="23"/>
+      <c r="AO46" s="23"/>
+      <c r="AP46" s="23"/>
+      <c r="AQ46" s="23"/>
+      <c r="AR46" s="23"/>
+      <c r="AS46" s="23"/>
+      <c r="AT46" s="23"/>
+      <c r="AU46" s="23"/>
+      <c r="AV46" s="23"/>
+      <c r="AW46" s="23"/>
+    </row>
+    <row r="47" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="AN47" s="23"/>
+      <c r="AO47" s="23"/>
+      <c r="AP47" s="23"/>
+      <c r="AQ47" s="23"/>
+      <c r="AR47" s="23"/>
+      <c r="AS47" s="23"/>
+      <c r="AT47" s="23"/>
+      <c r="AU47" s="23"/>
+      <c r="AV47" s="23"/>
+      <c r="AW47" s="23"/>
+      <c r="BA47" s="36"/>
+    </row>
+    <row r="48" spans="3:59" x14ac:dyDescent="0.35">
+      <c r="AN48" s="23"/>
+      <c r="AO48" s="23"/>
+      <c r="AP48" s="23"/>
+      <c r="AQ48" s="23"/>
+      <c r="AR48" s="23"/>
+      <c r="AS48" s="23"/>
+      <c r="AT48" s="23"/>
+      <c r="AU48" s="23"/>
+      <c r="AV48" s="23"/>
+      <c r="AW48" s="23"/>
+      <c r="BA48" s="36"/>
+    </row>
+    <row r="49" spans="3:49" x14ac:dyDescent="0.35">
+      <c r="AN49" s="23"/>
+      <c r="AO49" s="23"/>
+      <c r="AP49" s="23"/>
+      <c r="AQ49" s="23"/>
+      <c r="AR49" s="23"/>
+      <c r="AS49" s="23"/>
+      <c r="AT49" s="23"/>
+      <c r="AU49" s="23"/>
+      <c r="AV49" s="23"/>
+      <c r="AW49" s="23"/>
+    </row>
+    <row r="50" spans="3:49" x14ac:dyDescent="0.35">
+      <c r="C50" s="36"/>
+      <c r="AN50" s="23"/>
+      <c r="AO50" s="23"/>
+      <c r="AP50" s="23"/>
+      <c r="AQ50" s="23"/>
+      <c r="AR50" s="23"/>
+      <c r="AS50" s="23"/>
+      <c r="AT50" s="23"/>
+      <c r="AU50" s="23"/>
+      <c r="AV50" s="23"/>
+      <c r="AW50" s="23"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:AP34"/>

</xml_diff>

<commit_message>
update it in 200614
</commit_message>
<xml_diff>
--- a/learn_chinese.xlsx
+++ b/learn_chinese.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6223214-B3F6-4993-A576-6CB324DD7E81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AED68D-B482-4AC7-BC63-903DC9BBB8C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="27" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="28" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20190323" sheetId="1" r:id="rId1"/>
@@ -41,6 +41,7 @@
     <sheet name="20200516" sheetId="36" r:id="rId31"/>
     <sheet name="20200524" sheetId="37" r:id="rId32"/>
     <sheet name="20200531" sheetId="38" r:id="rId33"/>
+    <sheet name="20200614" sheetId="39" r:id="rId34"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="1936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="1998">
   <si>
     <t>1. Some simple chinese word</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45345,6 +45346,1790 @@
   </si>
   <si>
     <t>一千一百一十一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>做为我的股票经纪人，你怎么想。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: 如果他们做的很好，为什么还需要我的投资呢？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: 是什么呢？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: 有什么区别吗？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: 作为一个投资人，我是什么呢？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: 那就是你想做的吧，对吧？帮我买股票吧。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> As my stockbroker, what do you think?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: If they're doing so well, why do they need my investment?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A:And what are they.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A:What's the difference?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A:So what am I, as an investor?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: That's where you come in, right? Buying the stock for me.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dào nǐ bàn gōng shì 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rú guǒ tā men zuò de hěn hǎo ，wéi shen me hái xū yào wǒ de tóu zī ne ？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shì shí me ne ？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yǒu shen me qū bié ma ？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nà jiù shì nǐ xiǎng zuò de ba ，duì ba ？bāng wǒ mǎi gǔ piào ba 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 谢谢你能来，很抱歉，我没能</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>准时</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>到你办公室。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">xiè xiè nǐ néng lái ，hěn bào qiàn ，wǒ méi néng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">zhǔn shí </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 没关系，这对</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>股票经纪人</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>来说，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>是个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>寻常</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的时间，</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">méi guān xì ，zhè duì </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gǔ piào jīng jì rén</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lái shuō ，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bú</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> shì gè </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>xún cháng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de shí jiān ，</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>在说了</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，我们是老朋友了。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: That's all right. It's </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unusual</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>stockier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to keep these hours. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>And besides</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, you're an old friend.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>zài shuō le</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ，wǒ men shì lǎo péng yǒu le 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A:So, as I was saying. I think this might be a good time for me to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>invest in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>computer company</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 所以正如我所说的，这可能是我</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>投资</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>那家</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>电脑公司</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的好时机。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">suǒ yǐ zhèng rú wǒ suǒ shuō de ，zhè kě néng shì wǒ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tóu zī</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nà jiā </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>diàn nǎo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gōng sī</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de hǎo shí jī 。zuò wéi wǒ de gǔ piào jīng jì rén ，nǐ zěn me xiǎng 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 好吧，让我</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>稍微</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>解释</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>一下公司的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>财务</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B:All right. Let me </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>explain</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a little</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> abot corporate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>finance.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">hǎo ba ，ràng wǒ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shāo wēi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jiě shì </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">yī xià gōng sī de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cái wù</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 开始吧，当</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>涉及</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>到我的钱的时候，我非常感兴趣。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">kāi shǐ ba ，dāng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shè jí dào</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> wǒ de qián de shí hòu ，wǒ fēi cháng gǎn xìng qù 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 首先，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>公司企业</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要融资，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>特别是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>如果他们想要</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>扩张</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>shǒu xiān ，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gōng sī qǐ yè</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> xū yào róng zī ，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">tè bié shì </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">rú guǒ tā men xiǎng yào </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kuò zhāng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ，</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B;First of all, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>corporate enterprises</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, need financing, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>especially</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if they want to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>expand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Now, there are two </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">xiàn zài yǒu liǎng zhǒng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jī běn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de róng zī </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fāng shì</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>basic types</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of financing.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>现在有两种</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>基本</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的融资</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>方式</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>入股</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>举债</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Equity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>debt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rù gǔ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ，hé </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jǔ zhài</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>金钱的使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>由业主</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>提供</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的业务被称为股权融资，</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B:The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>use of money</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>supplied</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> by the owners of a business is called equity funding,  debt funding.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jīn qián de shǐ yòng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> yóu yè zhǔ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tí gòng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de yè wù bèi chēng wéi gǔ quán róng zī ，</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">zī jīn de shǐ yòng tí gòng de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dài kuǎn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bèi chēng wéi jǔ zhài róng zī 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">and the use of money supplied by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>loans</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is called debt funding</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>资金的使用提供的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>贷款</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>被称为举债融资。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B:Well, you become a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>partial owner</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the company and receive equity. </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 嗯， 你成为公司的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>部分所有者</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>并且获得股权。你可以得到</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> èn ， nǐ chéng wéi gōng sī de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bù fèn suǒ yǒu zhě</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bìng qiě huò dé gǔ quán 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You get shares of coommon stock to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>represent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> your portion of ownership.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>一些普通股票来</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>代表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>你的所有权。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nǐ kě yǐ dé dào yī xiē pǔ tōng gǔ piào lái </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dài biǎo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nǐ de suǒ yǒu quán</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: Thanks for coming over. I'm sorry I couldn't get to your office </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>on time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 我认为他们做的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>很好</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，他们可能会</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>欢迎</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>你的投资。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">wǒ rèn wéi tā men zuò de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hěn hǎo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ，tā men kě néng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>huì huān</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> yíng nǐ de tóu zī 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B:I think they're doing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> extremely well</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. And they would probably </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>welcome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> your investment.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A:Go ahead. When it </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>concerns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> my money, I'm very interested.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不同   bu tong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zuò wéi yī gè tóu zī rén ，wǒ shì shen me ne ？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -60972,7 +62757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{848D9323-1F0D-45DF-AADB-2E1BFD349A7F}">
   <dimension ref="C2:BA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="U47" sqref="U47"/>
     </sheetView>
   </sheetViews>
@@ -61345,6 +63130,395 @@
     <row r="47" spans="3:53" x14ac:dyDescent="0.35">
       <c r="D47" s="23" t="s">
         <v>1935</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B387F16-D0F5-4174-A352-C7602F9ABBAA}">
+  <dimension ref="C2:BA49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z35" sqref="Z35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.640625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="2.640625" style="23"/>
+    <col min="4" max="4" width="2.640625" style="23" customWidth="1"/>
+    <col min="5" max="8" width="2.640625" style="23"/>
+    <col min="9" max="9" width="2.7109375" style="23" customWidth="1"/>
+    <col min="10" max="15" width="2.640625" style="23"/>
+    <col min="16" max="16" width="2.640625" style="23" customWidth="1"/>
+    <col min="17" max="35" width="2.640625" style="23"/>
+    <col min="36" max="36" width="2.640625" style="23" customWidth="1"/>
+    <col min="37" max="38" width="2.640625" style="23"/>
+    <col min="39" max="39" width="2.640625" style="23" customWidth="1"/>
+    <col min="40" max="16384" width="2.640625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="C2" s="23" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="3" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="D3" s="23" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="4" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="C4" s="23" t="s">
+        <v>1954</v>
+      </c>
+      <c r="K4" s="32"/>
+      <c r="AB4" s="23" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="5" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="D5" s="23" t="s">
+        <v>1955</v>
+      </c>
+      <c r="K5" s="32"/>
+    </row>
+    <row r="6" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="E6" s="23" t="s">
+        <v>1949</v>
+      </c>
+      <c r="AM6" s="33"/>
+      <c r="AN6" s="32"/>
+    </row>
+    <row r="7" spans="3:40" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="23" t="s">
+        <v>1956</v>
+      </c>
+      <c r="AB7" s="23" t="s">
+        <v>1959</v>
+      </c>
+      <c r="AM7" s="33"/>
+      <c r="AN7" s="32"/>
+    </row>
+    <row r="8" spans="3:40" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="23" t="s">
+        <v>1958</v>
+      </c>
+      <c r="AM8" s="33"/>
+      <c r="AN8" s="32"/>
+    </row>
+    <row r="9" spans="3:40" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="23" t="s">
+        <v>1957</v>
+      </c>
+      <c r="AM9" s="33"/>
+      <c r="AN9" s="32"/>
+    </row>
+    <row r="10" spans="3:40" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="23" t="s">
+        <v>1960</v>
+      </c>
+      <c r="AM10" s="33"/>
+      <c r="AN10" s="32"/>
+    </row>
+    <row r="11" spans="3:40" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="23" t="s">
+        <v>1962</v>
+      </c>
+      <c r="AB11" s="23" t="s">
+        <v>1961</v>
+      </c>
+      <c r="AM11" s="33"/>
+      <c r="AN11" s="32"/>
+    </row>
+    <row r="12" spans="3:40" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="23" t="s">
+        <v>1937</v>
+      </c>
+      <c r="AC12" s="23" t="s">
+        <v>1943</v>
+      </c>
+      <c r="AM12" s="33"/>
+      <c r="AN12" s="32"/>
+    </row>
+    <row r="13" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="D13" s="23" t="s">
+        <v>1963</v>
+      </c>
+      <c r="J13" s="34"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="AM13" s="33"/>
+    </row>
+    <row r="14" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="D14" s="23" t="s">
+        <v>1964</v>
+      </c>
+      <c r="J14" s="34"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="AM14" s="33"/>
+    </row>
+    <row r="15" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="C15" s="23" t="s">
+        <v>1992</v>
+      </c>
+      <c r="AB15" s="23" t="s">
+        <v>1994</v>
+      </c>
+      <c r="AM15" s="33"/>
+      <c r="AN15" s="32"/>
+    </row>
+    <row r="16" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="D16" s="23" t="s">
+        <v>1993</v>
+      </c>
+      <c r="AM16" s="33"/>
+      <c r="AN16" s="32"/>
+    </row>
+    <row r="17" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="AM17" s="33"/>
+      <c r="AN17" s="32"/>
+    </row>
+    <row r="18" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="C18" s="23" t="s">
+        <v>1938</v>
+      </c>
+      <c r="AB18" s="23" t="s">
+        <v>1944</v>
+      </c>
+      <c r="AM18" s="33"/>
+    </row>
+    <row r="19" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="D19" s="23" t="s">
+        <v>1950</v>
+      </c>
+      <c r="AM19" s="33"/>
+    </row>
+    <row r="20" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="AM20" s="33"/>
+      <c r="AN20" s="32"/>
+    </row>
+    <row r="21" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="C21" s="23" t="s">
+        <v>1965</v>
+      </c>
+      <c r="AB21" s="23" t="s">
+        <v>1966</v>
+      </c>
+      <c r="AL21" s="32"/>
+    </row>
+    <row r="22" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="D22" s="23" t="s">
+        <v>1967</v>
+      </c>
+      <c r="AL22" s="32"/>
+    </row>
+    <row r="23" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="AL23" s="32"/>
+    </row>
+    <row r="24" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="C24" s="23" t="s">
+        <v>1968</v>
+      </c>
+      <c r="AB24" s="23" t="s">
+        <v>1995</v>
+      </c>
+      <c r="AL24" s="32"/>
+    </row>
+    <row r="25" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="D25" s="23" t="s">
+        <v>1969</v>
+      </c>
+      <c r="AL25" s="32"/>
+    </row>
+    <row r="26" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="C26" s="23" t="s">
+        <v>1970</v>
+      </c>
+      <c r="AB26" s="23" t="s">
+        <v>1972</v>
+      </c>
+      <c r="AL26" s="32"/>
+    </row>
+    <row r="27" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="C27" s="23" t="s">
+        <v>1975</v>
+      </c>
+      <c r="AC27" s="23" t="s">
+        <v>1974</v>
+      </c>
+      <c r="AL27" s="32"/>
+    </row>
+    <row r="28" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="D28" s="23" t="s">
+        <v>1971</v>
+      </c>
+      <c r="AL28" s="32"/>
+    </row>
+    <row r="29" spans="3:40" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="23" t="s">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="30" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="C30" s="23" t="s">
+        <v>1939</v>
+      </c>
+      <c r="AB30" s="23" t="s">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="31" spans="3:40" x14ac:dyDescent="0.35">
+      <c r="D31" s="23" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="33" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="C33" s="23" t="s">
+        <v>1976</v>
+      </c>
+      <c r="AB33" s="23" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="34" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="D34" s="23" t="s">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="35" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="C35" s="23" t="s">
+        <v>1940</v>
+      </c>
+      <c r="N35" s="23" t="s">
+        <v>1996</v>
+      </c>
+      <c r="AB35" s="23" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="36" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="D36" s="23" t="s">
+        <v>1952</v>
+      </c>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="32"/>
+      <c r="U36" s="32"/>
+      <c r="V36" s="32"/>
+      <c r="W36" s="32"/>
+      <c r="X36" s="32"/>
+      <c r="Y36" s="32"/>
+      <c r="Z36" s="32"/>
+      <c r="AA36" s="32"/>
+      <c r="AB36" s="32"/>
+      <c r="AC36" s="32"/>
+      <c r="AD36" s="32"/>
+      <c r="AE36" s="32"/>
+    </row>
+    <row r="37" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="C37" s="23" t="s">
+        <v>1979</v>
+      </c>
+      <c r="P37" s="32"/>
+      <c r="Q37" s="32"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="32"/>
+      <c r="T37" s="32"/>
+      <c r="U37" s="32"/>
+      <c r="V37" s="32"/>
+      <c r="W37" s="32"/>
+      <c r="X37" s="32"/>
+      <c r="Y37" s="32"/>
+      <c r="Z37" s="32"/>
+      <c r="AA37" s="32"/>
+      <c r="AB37" s="32" t="s">
+        <v>1980</v>
+      </c>
+      <c r="AC37" s="32"/>
+      <c r="AD37" s="32"/>
+      <c r="AE37" s="32"/>
+    </row>
+    <row r="38" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="D38" s="23" t="s">
+        <v>1984</v>
+      </c>
+      <c r="AC38" s="23" t="s">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="39" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="D39" s="23" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="40" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="D40" s="23" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="41" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="C41" s="23" t="s">
+        <v>1941</v>
+      </c>
+      <c r="AB41" s="23" t="s">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="42" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="D42" s="23" t="s">
+        <v>1997</v>
+      </c>
+      <c r="BA42" s="36"/>
+    </row>
+    <row r="43" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="BA43" s="36"/>
+    </row>
+    <row r="44" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="C44" s="23" t="s">
+        <v>1986</v>
+      </c>
+      <c r="AB44" s="23" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="45" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="C45" s="36"/>
+      <c r="D45" s="23" t="s">
+        <v>1989</v>
+      </c>
+      <c r="AB45" s="23" t="s">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="46" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="D46" s="23" t="s">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="47" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="D47" s="23" t="s">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="48" spans="3:53" x14ac:dyDescent="0.35">
+      <c r="C48" s="23" t="s">
+        <v>1942</v>
+      </c>
+      <c r="AB48" s="23" t="s">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D49" s="23" t="s">
+        <v>1953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the learn of 20200726
</commit_message>
<xml_diff>
--- a/learn_chinese.xlsx
+++ b/learn_chinese.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC80DB7-FE2E-4DAE-935A-4A389C74CD8A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4141CDB-6E5B-4AFC-846E-190CD3C0AFDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="32" activeTab="37" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="33" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20190323" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,8 @@
     <sheet name="20200621" sheetId="40" r:id="rId35"/>
     <sheet name="20200705" sheetId="41" r:id="rId36"/>
     <sheet name="20200712" sheetId="42" r:id="rId37"/>
-    <sheet name="20200719" sheetId="43" r:id="rId38"/>
+    <sheet name="20200719" sheetId="44" r:id="rId38"/>
+    <sheet name="20200726" sheetId="43" r:id="rId39"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2293" uniqueCount="2195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2360" uniqueCount="2259">
   <si>
     <t>1. Some simple chinese word</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52314,10 +52315,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Change root</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>wǎn shàng hǎo ，xiān shēng ，yǒu shen me xū yào bāng máng de ma ？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -52785,6 +52782,1471 @@
   </si>
   <si>
     <t>rú guǒ nín hái yǒu shen me bié de xū qiú ，qǐng gào sù wǒ men 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Change room</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buy food</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: 我来了，有什么需要我帮忙的？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: 给你，你还想要什么吗？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B; 当然可以。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: I'm coming, What can I do for you?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>told me to buy some for the neighbor.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">B: Yes. Let me show you. Eating more organically grown vegetables is good for </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: Here you are. Is there anything else you want?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: Sure.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nà zhēn shì hěn duō dōng xī ya ，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 早上好，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>有人在吗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>zǎo shàng hǎo ，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yǒu rén zài ma</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: Good moring.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Is anybody here</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 我想买一些</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>香蕉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，两块牛肉，一箱</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>低脂牛奶</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: I want to buy some </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>banana</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, two pieces of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>beef</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, a box of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>low fat milk</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">wǒ xiǎng mǎi yī xiē </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>xiāng jiāo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ，liǎng kuài </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>niú ròu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ，yī xiāng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dī zhī niú nǎi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ，</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2gōng jīn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jī dàn hé yī xiē shū cài 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>two kilos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of eggs and some vegetables.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2公斤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>鸡蛋和一些蔬菜。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 那真是很多东西呀，我可以给你找辆</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>购物车</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">wǒ kě yǐ gěi nǐ zhǎo liàng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gòu wù chē</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: That's quite a lot of things. I can find a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shopping cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for you.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 你人真好，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>苹果</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>多少钱？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>nǐ rén zhēn hǎo ，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>píng guǒ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> duō shǎo qián ？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: it's very nice of you. How much are the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>apples</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: Two for two dollars. You can go to the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fresh area</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Today's </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">liǎng měi yuán liǎng gè 。nǐ kě yǐ qù </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shēng xiān qū</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> kàn kàn ，</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">jīn tiān de shū cài </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bú jǐn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> xīn xiān ，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ér qiě</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tè jià 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 两美元两个。你可以去</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>生鲜区</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>看看，今天的蔬菜</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不仅</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>新鲜，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>而且</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>特价。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">vegetables are </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not only</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fresh </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>but also</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on sale.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nǐ hǎo ，nǐ men yǒu </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yǒu jī shū cài</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ma ？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 你好，你们有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>有机蔬菜</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>吗？我</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>丈夫</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>叫我买点给邻居。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: All right. Do you have any</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> organically grown vegetables</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">? My </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>husband</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>wǒ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zhàng fū</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jiào wǒ mǎi diǎn gěi lín jū 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 有啊，我带你去看看。多吃有机蔬菜对我们的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>健康</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>有好处，</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>有机蔬菜比普通蔬菜的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>营养成分高</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jiàn kāng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> yǒu hǎo chù, yǒu jī shū cài bǐ pǔ tōng shū cài de</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yíng yǎng chéng fèn gāo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">our </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>health</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. They are </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">more nutritious </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>than ordinary vegetables.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 是的，没错。但是他们有点</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>贵</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，给我一打土豆。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: yes, you are right. But they're a little </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>expensive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Give me a dozen potatoes.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">shì de ，méi cuò 。dàn shì tā men yǒu diǎn </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>guì</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ，</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 不了，谢谢，这些</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>一共</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>多少钱？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: No, thank you. How much are these </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in total</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">? </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">bú le ，xiè xiè ，zhè xiē </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yī gòng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> duō shǎo qián ？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 让我</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>算</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>一下，65美元。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ràng wǒ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>suàn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> yī xià ，65měi yuán 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: Let me </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>check</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Sixty-five dollars.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 我没有带现金，我能用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>信用卡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>支付吗？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>wǒ méi yǒu dài xiàn jīn ，wǒ néng yòng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> xìn yòng kǎ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>zhī fù ma ？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A; I have no cash with me. Can I  pay by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>credit card</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wǒ lái le ，yǒu shen me xū yào wǒ bāng máng de ？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>甜 ti</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>á</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n sweet</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>micrometer  千分尺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">家   jia   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>夫人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wife</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老公</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老婆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">husband </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">yǒu ā ，wǒ dài nǐ qù kàn kàn. duō chī yǒu jī shū cài duì wǒ men de </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gěi wǒ yī dá tǔ dòu 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gěi nǐ ，nǐ hái xiǎng yào shen me ma ？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">计算机 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -69931,11 +71393,11 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D66D7F4-F484-4491-BF10-3C4B71474B69}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF62A2C-3040-4BD3-8489-D3C754E2C9EE}">
   <dimension ref="C2:AD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.640625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -69960,7 +71422,7 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.35">
       <c r="D3" s="30" t="s">
-        <v>2183</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="4" spans="3:30" x14ac:dyDescent="0.35">
@@ -69973,7 +71435,7 @@
     </row>
     <row r="5" spans="3:30" x14ac:dyDescent="0.35">
       <c r="D5" s="23" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="6" spans="3:30" x14ac:dyDescent="0.35">
@@ -70025,15 +71487,15 @@
     </row>
     <row r="13" spans="3:30" x14ac:dyDescent="0.35">
       <c r="D13" s="23" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="14" spans="3:30" x14ac:dyDescent="0.35">
       <c r="C14" s="23" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
       <c r="AC14" s="23" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="15" spans="3:30" x14ac:dyDescent="0.35">
@@ -70046,7 +71508,7 @@
     </row>
     <row r="16" spans="3:30" x14ac:dyDescent="0.35">
       <c r="D16" s="23" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="17" spans="3:30" x14ac:dyDescent="0.35">
@@ -70064,10 +71526,10 @@
     </row>
     <row r="19" spans="3:30" x14ac:dyDescent="0.35">
       <c r="D19" s="23" t="s">
+        <v>2189</v>
+      </c>
+      <c r="AD19" s="23" t="s">
         <v>2190</v>
-      </c>
-      <c r="AD19" s="23" t="s">
-        <v>2191</v>
       </c>
     </row>
     <row r="20" spans="3:30" x14ac:dyDescent="0.35">
@@ -70085,7 +71547,7 @@
     </row>
     <row r="22" spans="3:30" x14ac:dyDescent="0.35">
       <c r="D22" s="23" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="23" spans="3:30" x14ac:dyDescent="0.35">
@@ -70124,7 +71586,7 @@
         <v>2179</v>
       </c>
       <c r="AC28" s="23" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="29" spans="3:30" x14ac:dyDescent="0.35">
@@ -70137,7 +71599,7 @@
         <v>2181</v>
       </c>
       <c r="AC30" s="23" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="31" spans="3:30" x14ac:dyDescent="0.35">
@@ -70168,7 +71630,330 @@
     </row>
     <row r="37" spans="3:29" x14ac:dyDescent="0.35">
       <c r="D37" s="23" t="s">
-        <v>2194</v>
+        <v>2193</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D66D7F4-F484-4491-BF10-3C4B71474B69}">
+  <dimension ref="C2:Y53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.640625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="2.640625" style="23"/>
+    <col min="4" max="4" width="2.640625" style="23" customWidth="1"/>
+    <col min="5" max="8" width="2.640625" style="23"/>
+    <col min="9" max="9" width="2.7109375" style="23" customWidth="1"/>
+    <col min="10" max="15" width="2.640625" style="23"/>
+    <col min="16" max="16" width="2.640625" style="23" customWidth="1"/>
+    <col min="17" max="35" width="2.640625" style="23"/>
+    <col min="36" max="36" width="2.640625" style="23" customWidth="1"/>
+    <col min="37" max="38" width="2.640625" style="23"/>
+    <col min="39" max="39" width="2.640625" style="23" customWidth="1"/>
+    <col min="40" max="16384" width="2.640625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="C2" s="23" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="3" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D3" s="30" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="4" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="C4" s="23" t="s">
+        <v>2205</v>
+      </c>
+      <c r="X4" s="23" t="s">
+        <v>2207</v>
+      </c>
+    </row>
+    <row r="5" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D5" s="23" t="s">
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="6" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="C6" s="23" t="s">
+        <v>2196</v>
+      </c>
+      <c r="X6" s="23" t="s">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="7" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D7" s="23" t="s">
+        <v>2246</v>
+      </c>
+    </row>
+    <row r="8" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="C8" s="23" t="s">
+        <v>2208</v>
+      </c>
+      <c r="X8" s="23" t="s">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="9" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D9" s="23" t="s">
+        <v>2213</v>
+      </c>
+      <c r="Y9" s="23" t="s">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="10" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D10" s="23" t="s">
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="11" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D11" s="23" t="s">
+        <v>2211</v>
+      </c>
+    </row>
+    <row r="12" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="C12" s="23" t="s">
+        <v>2214</v>
+      </c>
+      <c r="X12" s="23" t="s">
+        <v>2216</v>
+      </c>
+    </row>
+    <row r="13" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D13" s="23" t="s">
+        <v>2204</v>
+      </c>
+    </row>
+    <row r="14" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D14" s="23" t="s">
+        <v>2215</v>
+      </c>
+    </row>
+    <row r="15" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="C15" s="23" t="s">
+        <v>2217</v>
+      </c>
+      <c r="X15" s="23" t="s">
+        <v>2219</v>
+      </c>
+    </row>
+    <row r="16" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D16" s="23" t="s">
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="17" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="C17" s="23" t="s">
+        <v>2223</v>
+      </c>
+      <c r="X17" s="23" t="s">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="18" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D18" s="23" t="s">
+        <v>2224</v>
+      </c>
+      <c r="Y18" s="23" t="s">
+        <v>2225</v>
+      </c>
+    </row>
+    <row r="19" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D19" s="23" t="s">
+        <v>2221</v>
+      </c>
+    </row>
+    <row r="20" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D20" s="23" t="s">
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="21" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="C21" s="23" t="s">
+        <v>2227</v>
+      </c>
+      <c r="X21" s="23" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="22" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D22" s="23" t="s">
+        <v>2226</v>
+      </c>
+      <c r="Y22" s="23" t="s">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="23" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D23" s="23" t="s">
+        <v>2229</v>
+      </c>
+    </row>
+    <row r="24" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="C24" s="23" t="s">
+        <v>2230</v>
+      </c>
+      <c r="X24" s="23" t="s">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="25" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D25" s="23" t="s">
+        <v>2231</v>
+      </c>
+      <c r="Y25" s="23" t="s">
+        <v>2233</v>
+      </c>
+    </row>
+    <row r="26" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D26" s="23" t="s">
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="27" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D27" s="23" t="s">
+        <v>2232</v>
+      </c>
+    </row>
+    <row r="28" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="C28" s="23" t="s">
+        <v>2234</v>
+      </c>
+      <c r="X28" s="23" t="s">
+        <v>2235</v>
+      </c>
+    </row>
+    <row r="29" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D29" s="23" t="s">
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="30" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D30" s="23" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="31" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="C31" s="23" t="s">
+        <v>2197</v>
+      </c>
+      <c r="X31" s="23" t="s">
+        <v>2202</v>
+      </c>
+    </row>
+    <row r="32" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D32" s="23" t="s">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="34" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C34" s="23" t="s">
+        <v>2237</v>
+      </c>
+      <c r="X34" s="23" t="s">
+        <v>2238</v>
+      </c>
+    </row>
+    <row r="35" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D35" s="23" t="s">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="37" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C37" s="23" t="s">
+        <v>2240</v>
+      </c>
+      <c r="X37" s="23" t="s">
+        <v>2242</v>
+      </c>
+    </row>
+    <row r="38" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D38" s="23" t="s">
+        <v>2241</v>
+      </c>
+    </row>
+    <row r="40" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C40" s="23" t="s">
+        <v>2243</v>
+      </c>
+      <c r="X40" s="23" t="s">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="41" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D41" s="23" t="s">
+        <v>2244</v>
+      </c>
+    </row>
+    <row r="43" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C43" s="23" t="s">
+        <v>2198</v>
+      </c>
+      <c r="X43" s="23" t="s">
+        <v>2203</v>
+      </c>
+    </row>
+    <row r="44" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D44" s="23" t="s">
+        <v>2161</v>
+      </c>
+    </row>
+    <row r="47" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C47" s="23" t="s">
+        <v>2247</v>
+      </c>
+    </row>
+    <row r="48" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C48" s="23" t="s">
+        <v>2248</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C49" s="23" t="s">
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C50" s="23" t="s">
+        <v>2250</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C51" s="23" t="s">
+        <v>2252</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>2254</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C52" s="23" t="s">
+        <v>2253</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C53" s="23" t="s">
+        <v>2258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update it in 08/16
</commit_message>
<xml_diff>
--- a/learn_chinese.xlsx
+++ b/learn_chinese.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E613462-780F-4612-9AC0-3D7429722C3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB163BA-219F-4E29-B317-FE11A30B33C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="35" activeTab="40" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="36" activeTab="41" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20190323" sheetId="1" r:id="rId1"/>
@@ -49,6 +49,7 @@
     <sheet name="20200726" sheetId="43" r:id="rId39"/>
     <sheet name="20200802" sheetId="45" r:id="rId40"/>
     <sheet name="20200809" sheetId="46" r:id="rId41"/>
+    <sheet name="20200816" sheetId="47" r:id="rId42"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2471" uniqueCount="2367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2521" uniqueCount="2414">
   <si>
     <t>1. Some simple chinese word</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57323,6 +57324,1100 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> that your job will</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Happy birthday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: 这个派对真的很不错。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>比较搭配，希望我看起来就像自我感觉的那样好。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一起喝一杯。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I'm sure you'll have a good time.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: OK!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: This is a really wonderful party.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>your birthday.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhè gè pài duì zhēn de hěn bú cuò 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xiè xiè 。nǐ néng zhè me shuō zhēn shì tài hǎo le 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yī qǐ hē yī bēi 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>生日快乐</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>！这是给你的，brian。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shēng rì kuài lè</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ！zhè shì gěi nǐ de ，brian。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Happy birthday</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>! This is for you,Brian.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 我真高兴，你还</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>记得</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>我的生日。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">wǒ zhēn gāo xìng ，nǐ hái </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jì dé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> wǒ de shēng rì 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">三生有幸 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">sān shēng yǒu xìng </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">shì de ，nǐ zǒng shì hěn </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shòu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dà jiā </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>huān yíng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>nǐ jīn tiān kàn shàng qù hěn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> piāo liàng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: Yes. You are always </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>popular</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with everyone. And you look very </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pretty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> today.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 是的，你总是很</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>受</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>大家</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>欢迎</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。你今天看上去很</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>漂亮</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沉鱼落雁，闭月羞花。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chén yú luò yàn ，bì yuè xiū huā 。</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: Thanks. That's kind of you to say so. I hope my </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>necklace</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> goes with my </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 谢谢。你能这么说真是太好了。我希望我的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>项链</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>衣服</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dress</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and they both make me looks good as I feel.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>wǒ xī wàng wǒ de</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> xiàng liàn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hé </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yī fú</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bǐ jiào dā pèi ，</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 你看上去不错，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>绝对</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>光芒四射</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: You look great. You're </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>absolutily</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>glowing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>nǐ kàn shàng qù bú cuò ，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">jué duì </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">shì </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>guāng máng sì shè</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">wǒ men yīng gāi wéi </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>qìng zhù</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nǐ de shēng rì</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>快进来，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>大家</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>都在，我肯定你会玩的很高兴的。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: I'm so happy you </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>remembered</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Please come in. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Everyone</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is here.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>kuài jìn lái ，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dà jiā</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dōu zài ，wǒ kěn dìng nǐ huì wán de hěn gāo xìng de 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: Brian，能</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>有幸</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>和你跳个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>舞</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>吗？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: Brian, May I </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>have the pleasure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to have a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with you?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Brian，néng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yǒu xìng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hé nǐ tiào gè</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> wǔ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ma ？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>她有沉鱼落雁，闭月羞花之姿。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tā yǒu chén yú luò yàn ，bì yuè xiū huā zhī zī 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>xī wàng wǒ kàn qǐ lái jiù xiàng zì wǒ gǎn ju</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>é</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de nà yàng hǎo 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相对</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>relatively</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xiang dui</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 谢谢，这个派对真</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>有趣</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。我们应该为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>庆祝</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>你的生日</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: Thanks. This is a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fun</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Party. We should have a drink together to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>celebrate</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">xiè xiè ，zhè gè pài duì zhēn </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yǒu qù</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -76110,8 +77205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B4C166-06FC-4512-952F-3AA4BF3842BA}">
   <dimension ref="C2:Z40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.640625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -76348,6 +77443,256 @@
     <row r="40" spans="3:25" x14ac:dyDescent="0.35">
       <c r="D40" s="23" t="s">
         <v>2326</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08DB7238-2225-4047-819A-A375E53021ED}">
+  <dimension ref="C2:AB47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X43" sqref="X43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.640625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="2.640625" style="23"/>
+    <col min="4" max="4" width="2.640625" style="23" customWidth="1"/>
+    <col min="5" max="8" width="2.640625" style="23"/>
+    <col min="9" max="9" width="2.7109375" style="23" customWidth="1"/>
+    <col min="10" max="15" width="2.640625" style="23"/>
+    <col min="16" max="16" width="2.640625" style="23" customWidth="1"/>
+    <col min="17" max="36" width="2.640625" style="23"/>
+    <col min="37" max="37" width="2.640625" style="23" customWidth="1"/>
+    <col min="38" max="39" width="2.640625" style="23"/>
+    <col min="40" max="40" width="2.640625" style="23" customWidth="1"/>
+    <col min="41" max="16384" width="2.640625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="C2" s="23" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="3" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D3" s="30" t="s">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="4" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="C4" s="23" t="s">
+        <v>2378</v>
+      </c>
+      <c r="AA4" s="23" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="5" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D5" s="23" t="s">
+        <v>2379</v>
+      </c>
+    </row>
+    <row r="6" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="C6" s="23" t="s">
+        <v>2381</v>
+      </c>
+      <c r="AA6" s="23" t="s">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="7" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D7" s="23" t="s">
+        <v>2399</v>
+      </c>
+      <c r="AB7" s="23" t="s">
+        <v>2371</v>
+      </c>
+    </row>
+    <row r="8" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D8" s="23" t="s">
+        <v>2382</v>
+      </c>
+    </row>
+    <row r="9" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D9" s="23" t="s">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="10" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="C10" s="23" t="s">
+        <v>2402</v>
+      </c>
+      <c r="AA10" s="23" t="s">
+        <v>2403</v>
+      </c>
+    </row>
+    <row r="11" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D11" s="23" t="s">
+        <v>2404</v>
+      </c>
+    </row>
+    <row r="13" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="C13" s="23" t="s">
+        <v>1882</v>
+      </c>
+      <c r="AA13" s="23" t="s">
+        <v>2372</v>
+      </c>
+    </row>
+    <row r="14" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D14" s="23" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="16" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="C16" s="23" t="s">
+        <v>2368</v>
+      </c>
+      <c r="AA16" s="23" t="s">
+        <v>2373</v>
+      </c>
+    </row>
+    <row r="17" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D17" s="23" t="s">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="19" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="C19" s="23" t="s">
+        <v>2388</v>
+      </c>
+      <c r="AA19" s="23" t="s">
+        <v>2387</v>
+      </c>
+    </row>
+    <row r="20" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D20" s="23" t="s">
+        <v>2385</v>
+      </c>
+    </row>
+    <row r="21" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D21" s="23" t="s">
+        <v>2386</v>
+      </c>
+    </row>
+    <row r="22" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="C22" s="23" t="s">
+        <v>2392</v>
+      </c>
+      <c r="AA22" s="23" t="s">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="23" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D23" s="23" t="s">
+        <v>2369</v>
+      </c>
+      <c r="AB23" s="23" t="s">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="24" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D24" s="23" t="s">
+        <v>2376</v>
+      </c>
+    </row>
+    <row r="25" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D25" s="23" t="s">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="26" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D26" s="23" t="s">
+        <v>2407</v>
+      </c>
+    </row>
+    <row r="27" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="C27" s="23" t="s">
+        <v>2395</v>
+      </c>
+      <c r="AA27" s="23" t="s">
+        <v>2396</v>
+      </c>
+    </row>
+    <row r="28" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D28" s="23" t="s">
+        <v>2397</v>
+      </c>
+    </row>
+    <row r="30" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="C30" s="23" t="s">
+        <v>2411</v>
+      </c>
+      <c r="AA30" s="23" t="s">
+        <v>2412</v>
+      </c>
+    </row>
+    <row r="31" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D31" s="23" t="s">
+        <v>2370</v>
+      </c>
+      <c r="AB31" s="23" t="s">
+        <v>2374</v>
+      </c>
+    </row>
+    <row r="32" spans="3:28" x14ac:dyDescent="0.35">
+      <c r="D32" s="23" t="s">
+        <v>2413</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="D33" s="23" t="s">
+        <v>2398</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="D34" s="23" t="s">
+        <v>2377</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C38" s="23" t="s">
+        <v>2383</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>2384</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C40" s="23" t="s">
+        <v>2389</v>
+      </c>
+      <c r="K40" s="23" t="s">
+        <v>2390</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C42" s="23" t="s">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C43" s="23" t="s">
+        <v>2406</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C46" s="23" t="s">
+        <v>2408</v>
+      </c>
+      <c r="F46" s="23" t="s">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="47" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C47" s="23" t="s">
+        <v>2410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update it in 20200830
</commit_message>
<xml_diff>
--- a/learn_chinese.xlsx
+++ b/learn_chinese.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648EDE30-15E8-4FC6-B662-30EAC3076512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26522E44-8A42-46DA-9A69-B145F41BC88C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="37" activeTab="42" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="38" activeTab="43" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20190323" sheetId="1" r:id="rId1"/>
@@ -51,6 +51,7 @@
     <sheet name="20200809" sheetId="46" r:id="rId41"/>
     <sheet name="20200816" sheetId="47" r:id="rId42"/>
     <sheet name="20200823" sheetId="48" r:id="rId43"/>
+    <sheet name="20200830" sheetId="49" r:id="rId44"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2564" uniqueCount="2456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2630" uniqueCount="2521">
   <si>
     <t>1. Some simple chinese word</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59192,6 +59193,1147 @@
   </si>
   <si>
     <t>路人皆知.“司马昭之心，路人皆知”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: Jack, 你在干什么？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: 你知道你不应该那么做，我已经和你说过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很多次了，这对你没好处。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这里玩一整天。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: 但它真的很有趣，而且我并没有觉得有什么问题。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你不知道吗？你现在应该立刻去写作业。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: 我可不这么认为，你的老师之前告诉我，你这次期末考试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: 可是我现在只想玩这个。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>才能玩这个。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: 请在给我5分钟时间。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: 不行。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: Jack, what are you doing?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: you know, you shouldn't do that. I've told you so many times.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>it's not good for you.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: But it was really fun and I didn't think there was anything wrong with it.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>of this. Don't you know. You should do your homework right now.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: But that's all I want to do right now.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: I said no. and I also said that you can play this only if you have done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>what you should do.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B: Please give me another five minutes.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A: No way.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Jack, nǐ zài gàn sh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>é</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n me ？</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nǐ zhī dào nǐ bú yīng gāi nà me zuò ，wǒ yǐ jīng hé nǐ shuō guò</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hěn duō cì le ，zhè duì nǐ méi hǎo chù</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">dàn shì wǒ hěn xǐ huān ā ，zhēn de hěn yǒu qù ，wǒ hěn xiǎng zài </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhè lǐ wán yī zhěng tiān.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nǐ xiǎng tài duō le ，nǐ xǐ huān tā ，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dàn tā zhēn de hěn yǒu qù ，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">nǐ bú zhī dào ma ？nǐ xiàn zài yīng gāi lì kè qù xiě zuò yè 。	</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wǒ kě bú zhè me rèn wéi ，nǐ de lǎo shī zhī qián gào sù wǒ ，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nǐ cuò le ，wǒ xué huì le nà xiē zhī shí ，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">kě shì wǒ xiàn zài zhī xiǎng wán zhè gè </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wǒ shuō le bú xing ，ér qiě wǒ zhī qián shuō guò ，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qǐng zài gěi wǒ 5fèn zhōng shí jiān 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>bú x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Í</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 我在玩</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>泥巴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: I'm playing with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mud</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">wǒ zài wán </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ní bā</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 但是我很喜欢啊，真的很</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>有趣</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，我很想在</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: But I love it. It's really </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>interesting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. I love to play it all day.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 你玩这个是没有问题，但是你因为玩这个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>成绩</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>都下降了，</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nǐ wán zhè gè shì méi yǒu wèn tí, dàn shì nǐ yīn wéi wán zhè gè </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">chéng jì </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dōu xià jiàng le</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: There's no problem with you playing this. But your </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>score</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is down because</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 那个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>太无聊了</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，我已经把所有的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>都学会了。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: That's </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>boring</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. I've learned all the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>knowledge</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nà gè </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tài wú liáo le</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ，wǒ yǐ jīng bǎ suǒ yǒu de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">zhī shi </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dōu xué huì le 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: I don't think so. Your teacher told me that you </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cheated</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on the final exam </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>nǐ zhè cì qī mò kǎo shì</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zuò bì</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> le ，zhè </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">shuō míng </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">which </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>means</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> you don't know anything about it.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nǐ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gēn běn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dōu bú huì nà xiē zhī shí 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>作弊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>了，这</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>说明</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>你</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>根本</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>都不会那些知识。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B: 你错了，我学会了那些知识，我只是不想动</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>脑子</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>计算。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B: You're wrong. I've learned that knowledge. I just don't want to use my </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>brain</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">wǒ zhī shì bú xiǎng dòng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nǎo zǐ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jì suàn 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 你个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>骗子</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，赶紧停下来去写你的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>作业</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A; You're a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>liar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Stop and write your </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>homework</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nǐ gè </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">piàn zǐ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">，gǎn jǐn tíng xià lái qù xiě nǐ de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">zuò yè </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 你想太多了，你喜欢它，并不</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>意味着</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>你能这样做。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>bìng bú</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> yì wèi zhe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nǐ néng zhè yàng zuò </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A: You think too much. You like it doesn't </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mean</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> you can do it.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>ér qiě wǒ bìng méi yǒu ji</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Ú</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dé yǒu shen me wèn tí 。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A: 我说了不行，而且我之前说过，你</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>只有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>把你应该做的做好</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>nǐ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zhī yǒu </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bǎ nǐ yīng gāi zuò de zuò hǎo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">cái </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">néng wán zhè gè </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没门儿</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -78479,7 +79621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57975C92-21AA-4F03-8CF4-A8EA6AD61109}">
   <dimension ref="C2:AA34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
@@ -78677,6 +79819,327 @@
     <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="23" t="s">
         <v>2455</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C46A55A-007C-4655-AA87-4CA93348920E}">
+  <dimension ref="C2:X53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA53" sqref="AA53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.640625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="2.640625" style="23"/>
+    <col min="4" max="4" width="2.640625" style="23" customWidth="1"/>
+    <col min="5" max="8" width="2.640625" style="23"/>
+    <col min="9" max="9" width="2.7109375" style="23" customWidth="1"/>
+    <col min="10" max="15" width="2.640625" style="23"/>
+    <col min="16" max="16" width="2.640625" style="23" customWidth="1"/>
+    <col min="17" max="36" width="2.640625" style="23"/>
+    <col min="37" max="37" width="2.640625" style="23" customWidth="1"/>
+    <col min="38" max="39" width="2.640625" style="23"/>
+    <col min="40" max="40" width="2.640625" style="23" customWidth="1"/>
+    <col min="41" max="16384" width="2.640625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C2" s="23" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="3" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D3" s="30"/>
+    </row>
+    <row r="4" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C4" s="23" t="s">
+        <v>2456</v>
+      </c>
+      <c r="W4" s="23" t="s">
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="5" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D5" s="23" t="s">
+        <v>2477</v>
+      </c>
+    </row>
+    <row r="7" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C7" s="23" t="s">
+        <v>2491</v>
+      </c>
+      <c r="W7" s="23" t="s">
+        <v>2492</v>
+      </c>
+    </row>
+    <row r="8" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D8" s="23" t="s">
+        <v>2493</v>
+      </c>
+    </row>
+    <row r="10" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C10" s="23" t="s">
+        <v>2457</v>
+      </c>
+      <c r="W10" s="23" t="s">
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="11" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D11" s="23" t="s">
+        <v>2458</v>
+      </c>
+      <c r="X11" s="23" t="s">
+        <v>2469</v>
+      </c>
+    </row>
+    <row r="12" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D12" s="23" t="s">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="13" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D13" s="23" t="s">
+        <v>2479</v>
+      </c>
+    </row>
+    <row r="14" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C14" s="23" t="s">
+        <v>2494</v>
+      </c>
+      <c r="W14" s="23" t="s">
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="15" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D15" s="23" t="s">
+        <v>2459</v>
+      </c>
+    </row>
+    <row r="16" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D16" s="23" t="s">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="17" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D17" s="23" t="s">
+        <v>2481</v>
+      </c>
+    </row>
+    <row r="18" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C18" s="23" t="s">
+        <v>2513</v>
+      </c>
+      <c r="W18" s="23" t="s">
+        <v>2515</v>
+      </c>
+    </row>
+    <row r="19" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D19" s="23" t="s">
+        <v>2482</v>
+      </c>
+    </row>
+    <row r="20" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D20" s="23" t="s">
+        <v>2514</v>
+      </c>
+    </row>
+    <row r="21" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C21" s="23" t="s">
+        <v>2460</v>
+      </c>
+      <c r="W21" s="23" t="s">
+        <v>2470</v>
+      </c>
+    </row>
+    <row r="22" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D22" s="23" t="s">
+        <v>2483</v>
+      </c>
+    </row>
+    <row r="23" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D23" s="23" t="s">
+        <v>2516</v>
+      </c>
+    </row>
+    <row r="24" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C24" s="23" t="s">
+        <v>2496</v>
+      </c>
+      <c r="W24" s="23" t="s">
+        <v>2498</v>
+      </c>
+    </row>
+    <row r="25" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D25" s="23" t="s">
+        <v>2461</v>
+      </c>
+      <c r="X25" s="23" t="s">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="26" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D26" s="23" t="s">
+        <v>2497</v>
+      </c>
+    </row>
+    <row r="27" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D27" s="23" t="s">
+        <v>2484</v>
+      </c>
+    </row>
+    <row r="28" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C28" s="23" t="s">
+        <v>2499</v>
+      </c>
+      <c r="W28" s="23" t="s">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="29" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D29" s="23" t="s">
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="31" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C31" s="23" t="s">
+        <v>2462</v>
+      </c>
+      <c r="W31" s="23" t="s">
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="32" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D32" s="23" t="s">
+        <v>2506</v>
+      </c>
+      <c r="X32" s="23" t="s">
+        <v>2504</v>
+      </c>
+    </row>
+    <row r="33" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D33" s="23" t="s">
+        <v>2485</v>
+      </c>
+    </row>
+    <row r="34" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D34" s="23" t="s">
+        <v>2503</v>
+      </c>
+    </row>
+    <row r="35" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D35" s="23" t="s">
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="36" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C36" s="23" t="s">
+        <v>2507</v>
+      </c>
+      <c r="W36" s="23" t="s">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="37" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D37" s="23" t="s">
+        <v>2486</v>
+      </c>
+    </row>
+    <row r="38" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D38" s="23" t="s">
+        <v>2509</v>
+      </c>
+    </row>
+    <row r="39" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C39" s="23" t="s">
+        <v>2510</v>
+      </c>
+      <c r="W39" s="23" t="s">
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="40" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D40" s="23" t="s">
+        <v>2512</v>
+      </c>
+    </row>
+    <row r="42" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C42" s="23" t="s">
+        <v>2463</v>
+      </c>
+      <c r="W42" s="23" t="s">
+        <v>2472</v>
+      </c>
+    </row>
+    <row r="43" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D43" s="23" t="s">
+        <v>2487</v>
+      </c>
+    </row>
+    <row r="45" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="C45" s="23" t="s">
+        <v>2517</v>
+      </c>
+      <c r="W45" s="23" t="s">
+        <v>2473</v>
+      </c>
+    </row>
+    <row r="46" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D46" s="23" t="s">
+        <v>2464</v>
+      </c>
+      <c r="X46" s="23" t="s">
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="47" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D47" s="23" t="s">
+        <v>2488</v>
+      </c>
+    </row>
+    <row r="48" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="D48" s="23" t="s">
+        <v>2518</v>
+      </c>
+    </row>
+    <row r="49" spans="3:23" x14ac:dyDescent="0.35">
+      <c r="C49" s="23" t="s">
+        <v>2465</v>
+      </c>
+      <c r="W49" s="23" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="50" spans="3:23" x14ac:dyDescent="0.35">
+      <c r="D50" s="23" t="s">
+        <v>2489</v>
+      </c>
+    </row>
+    <row r="52" spans="3:23" x14ac:dyDescent="0.35">
+      <c r="C52" s="23" t="s">
+        <v>2466</v>
+      </c>
+      <c r="G52" s="23" t="s">
+        <v>2520</v>
+      </c>
+      <c r="W52" s="23" t="s">
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="53" spans="3:23" x14ac:dyDescent="0.35">
+      <c r="D53" s="23" t="s">
+        <v>2490</v>
+      </c>
+      <c r="G53" s="23" t="s">
+        <v>2519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>